<commit_message>
Writing note 010 fixed typos etc.
</commit_message>
<xml_diff>
--- a/resources/analysis/grammar/Features.xlsx
+++ b/resources/analysis/grammar/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j\resources\analysis\grammar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8CEBBA-D40F-4DFC-AA2E-997A8A41F26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F2F7D3-DCAB-42BA-AB77-02811542532B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2509" uniqueCount="321">
   <si>
     <t>Page</t>
   </si>
@@ -1005,6 +1005,44 @@
   <si>
     <t>Language A</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Characters here use the Slot alphabet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-B-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1013,7 +1051,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1144,6 +1182,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1728,7 +1781,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
@@ -1759,27 +1812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1789,47 +1821,17 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1846,6 +1848,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -49200,96 +49259,96 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20:U21"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="36"/>
-    <col min="2" max="2" width="9.140625" style="38"/>
+    <col min="1" max="1" width="9.140625" style="21"/>
+    <col min="2" max="2" width="9.140625" style="23"/>
     <col min="3" max="7" width="9.140625" style="15"/>
-    <col min="8" max="8" width="9.140625" style="36"/>
-    <col min="9" max="9" width="9.140625" style="38"/>
-    <col min="15" max="15" width="9.140625" style="36"/>
+    <col min="8" max="8" width="9.140625" style="21"/>
+    <col min="9" max="9" width="9.140625" style="23"/>
+    <col min="15" max="15" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="45"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="I1" s="45"/>
+    <row r="1" spans="2:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="I1" s="28"/>
     </row>
-    <row r="2" spans="2:14" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="I2" s="45"/>
+    <row r="2" spans="2:14" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="28"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="26" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="20" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="34" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="35" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="41" t="s">
-        <v>55</v>
+    <row r="5" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="46" t="s">
+        <v>320</v>
       </c>
       <c r="C5" s="10">
         <v>7.0013135943978889E-3</v>
@@ -49306,15 +49365,15 @@
       <c r="G5" s="11">
         <v>1.687311539424638E-2</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="17"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="10">
@@ -49332,7 +49391,7 @@
       <c r="G6" s="11">
         <v>1.2580608743783141E-2</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I6" s="24" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="7">
@@ -49352,7 +49411,7 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="10">
@@ -49370,7 +49429,7 @@
       <c r="G7" s="11">
         <v>2.8726450704681186E-2</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="25" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="7">
@@ -49390,7 +49449,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="25" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="10">
@@ -49408,7 +49467,7 @@
       <c r="G8" s="11">
         <v>0.14833541139961606</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="7">
@@ -49428,7 +49487,7 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="10">
@@ -49446,7 +49505,7 @@
       <c r="G9" s="11">
         <v>3.0261849614427731E-2</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="25" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="7">
@@ -49466,7 +49525,7 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="10">
@@ -49484,7 +49543,7 @@
       <c r="G10" s="11">
         <v>3.7961392258560801E-2</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="25" t="s">
         <v>35</v>
       </c>
       <c r="J10" s="7">
@@ -49504,7 +49563,7 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="10">
@@ -49522,7 +49581,7 @@
       <c r="G11" s="11">
         <v>4.7836739517217675E-2</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="25" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="7">
@@ -49542,7 +49601,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="26" t="s">
         <v>316</v>
       </c>
       <c r="C12" s="10">
@@ -49560,7 +49619,7 @@
       <c r="G12" s="11">
         <v>1.8728994112941162E-2</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="25" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="7">
@@ -49580,7 +49639,7 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="10">
@@ -49598,7 +49657,7 @@
       <c r="G13" s="11">
         <v>4.1683812916798362E-3</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="25" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="7">
@@ -49618,7 +49677,7 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="10">
@@ -49636,7 +49695,7 @@
       <c r="G14" s="11">
         <v>0.12612652085158385</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="25" t="s">
         <v>32</v>
       </c>
       <c r="J14" s="7">
@@ -49656,7 +49715,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="10">
@@ -49674,7 +49733,7 @@
       <c r="G15" s="11">
         <v>6.0064831503101955E-2</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="25" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="7">
@@ -49694,7 +49753,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="10">
@@ -49712,7 +49771,7 @@
       <c r="G16" s="11">
         <v>6.8392740874564817E-2</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="25" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="7">
@@ -49732,7 +49791,7 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="10">
@@ -49750,7 +49809,7 @@
       <c r="G17" s="11">
         <v>2.5901016939680287E-2</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="26" t="s">
         <v>315</v>
       </c>
       <c r="J17" s="7">
@@ -49770,7 +49829,7 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="10">
@@ -49788,7 +49847,7 @@
       <c r="G18" s="11">
         <v>8.5663309588818737E-3</v>
       </c>
-      <c r="I18" s="42" t="s">
+      <c r="I18" s="25" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="7">
@@ -49808,7 +49867,7 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="10">
@@ -49826,7 +49885,7 @@
       <c r="G19" s="11">
         <v>7.307505772441035E-2</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="26" t="s">
         <v>313</v>
       </c>
       <c r="J19" s="7">
@@ -49846,7 +49905,7 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="25" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="10">
@@ -49864,7 +49923,7 @@
       <c r="G20" s="11">
         <v>2.5059251764573492E-2</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="25" t="s">
         <v>61</v>
       </c>
       <c r="J20" s="7">
@@ -49884,7 +49943,7 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="10">
@@ -49902,7 +49961,7 @@
       <c r="G21" s="11">
         <v>0.10350592016679219</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="I21" s="25" t="s">
         <v>47</v>
       </c>
       <c r="J21" s="7">
@@ -49922,7 +49981,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="10">
@@ -49940,7 +49999,7 @@
       <c r="G22" s="11">
         <v>2.71530870964505E-2</v>
       </c>
-      <c r="I22" s="42" t="s">
+      <c r="I22" s="25" t="s">
         <v>49</v>
       </c>
       <c r="J22" s="7">
@@ -49960,7 +50019,7 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="10">
@@ -49978,7 +50037,7 @@
       <c r="G23" s="11">
         <v>4.8226608244051365E-3</v>
       </c>
-      <c r="I23" s="42" t="s">
+      <c r="I23" s="25" t="s">
         <v>48</v>
       </c>
       <c r="J23" s="7">
@@ -49998,7 +50057,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="10">
@@ -50016,7 +50075,7 @@
       <c r="G24" s="11">
         <v>1.0379361408645885E-2</v>
       </c>
-      <c r="I24" s="42" t="s">
+      <c r="I24" s="25" t="s">
         <v>60</v>
       </c>
       <c r="J24" s="7">
@@ -50036,7 +50095,7 @@
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="10">
@@ -50054,7 +50113,7 @@
       <c r="G25" s="11">
         <v>6.8256451969409632E-2</v>
       </c>
-      <c r="I25" s="42" t="s">
+      <c r="I25" s="25" t="s">
         <v>50</v>
       </c>
       <c r="J25" s="7">
@@ -50074,7 +50133,7 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="10">
@@ -50092,7 +50151,7 @@
       <c r="G26" s="11">
         <v>0.2567223191711816</v>
       </c>
-      <c r="I26" s="42" t="s">
+      <c r="I26" s="25" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="7">
@@ -50112,7 +50171,7 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="25" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="10">
@@ -50130,7 +50189,7 @@
       <c r="G27" s="11">
         <v>1.2236038885085398E-2</v>
       </c>
-      <c r="I27" s="42" t="s">
+      <c r="I27" s="25" t="s">
         <v>40</v>
       </c>
       <c r="J27" s="7">
@@ -50150,7 +50209,7 @@
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="10">
@@ -50168,7 +50227,7 @@
       <c r="G28" s="11">
         <v>2.5091783494684862E-2</v>
       </c>
-      <c r="I28" s="42" t="s">
+      <c r="I28" s="25" t="s">
         <v>37</v>
       </c>
       <c r="J28" s="7">
@@ -50188,7 +50247,7 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="10">
@@ -50206,7 +50265,7 @@
       <c r="G29" s="11">
         <v>4.2239943422294627E-3</v>
       </c>
-      <c r="I29" s="42" t="s">
+      <c r="I29" s="25" t="s">
         <v>53</v>
       </c>
       <c r="J29" s="7">
@@ -50226,7 +50285,7 @@
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="10">
@@ -50244,7 +50303,7 @@
       <c r="G30" s="11">
         <v>5.2972194706273672E-2</v>
       </c>
-      <c r="I30" s="42" t="s">
+      <c r="I30" s="25" t="s">
         <v>52</v>
       </c>
       <c r="J30" s="7">
@@ -50264,7 +50323,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="10">
@@ -50282,7 +50341,7 @@
       <c r="G31" s="11">
         <v>1.4087098251719552E-2</v>
       </c>
-      <c r="I31" s="42" t="s">
+      <c r="I31" s="25" t="s">
         <v>7</v>
       </c>
       <c r="J31" s="7">
@@ -50302,7 +50361,7 @@
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="10">
@@ -50320,7 +50379,7 @@
       <c r="G32" s="11">
         <v>6.4267269125070853E-3</v>
       </c>
-      <c r="I32" s="42" t="s">
+      <c r="I32" s="25" t="s">
         <v>21</v>
       </c>
       <c r="J32" s="7">
@@ -50340,7 +50399,7 @@
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="26" t="s">
         <v>314</v>
       </c>
       <c r="C33" s="10">
@@ -50358,7 +50417,7 @@
       <c r="G33" s="11">
         <v>5.9311757011703704E-3</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="25" t="s">
         <v>23</v>
       </c>
       <c r="J33" s="7">
@@ -50378,7 +50437,7 @@
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="10">
@@ -50396,7 +50455,7 @@
       <c r="G34" s="11">
         <v>0.22898454237132829</v>
       </c>
-      <c r="I34" s="42" t="s">
+      <c r="I34" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="7">
@@ -50416,7 +50475,7 @@
       </c>
     </row>
     <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="13">
@@ -50434,7 +50493,7 @@
       <c r="G35" s="14">
         <v>9.3077326444290804E-3</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="I35" s="27" t="s">
         <v>24</v>
       </c>
       <c r="J35" s="8">
@@ -50453,41 +50512,43 @@
         <v>7.9554304043853476E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:14" s="36" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="45"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="I36" s="45"/>
+    <row r="36" spans="2:14" s="21" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="28"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="I36" s="28"/>
     </row>
-    <row r="37" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="45"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="I37" s="45"/>
+    <row r="37" spans="2:14" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="47" t="s">
+        <v>319</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="I37" s="28"/>
     </row>
-    <row r="38" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="45"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="I38" s="45"/>
+    <row r="38" spans="2:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="28"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="I38" s="28"/>
     </row>
-    <row r="39" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="45"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="I39" s="45"/>
+    <row r="39" spans="2:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="28"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="I39" s="28"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G65">
@@ -50519,6 +50580,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>